<commit_message>
capitalization fixes for NonGeoLookupTables
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/NonGeoLookupTables.xlsx
+++ b/FME_files/LOOKUP_TABLES/NonGeoLookupTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7913F9A6-EB70-4C0C-A23C-93C942C4D262}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA98F4F-2418-45D8-851C-0ED6A9BB6C71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="7350" windowWidth="19580" windowHeight="11110" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25965" yWindow="17700" windowWidth="22710" windowHeight="14445" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format_TBS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="137">
   <si>
     <t>TBS_value</t>
   </si>
@@ -294,9 +294,6 @@
     <t>guide</t>
   </si>
   <si>
-    <t>province_Code</t>
-  </si>
-  <si>
     <t>TBS_topic</t>
   </si>
   <si>
@@ -403,6 +400,54 @@
   </si>
   <si>
     <t>never</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>txt</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>docx</t>
+  </si>
+  <si>
+    <t>xls</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>application/msaccess</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>technical_document</t>
+  </si>
+  <si>
+    <t>data_dictionary</t>
+  </si>
+  <si>
+    <t>information</t>
   </si>
 </sst>
 </file>
@@ -720,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C46"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1239,6 +1284,138 @@
         <v>50</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>128</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>131</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1248,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589F8EF7-A369-418C-AD91-10E8DD305FDA}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1442,7 +1619,7 @@
         <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1453,7 +1630,7 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1464,7 +1641,7 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1475,29 +1652,29 @@
         <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1508,40 +1685,40 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
         <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1552,29 +1729,29 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29" t="s">
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1584,15 +1761,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DA827-7F8F-427A-89AE-B21D8717466C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
     <col min="2" max="2" width="14.90625" customWidth="1"/>
     <col min="3" max="3" width="15.453125" customWidth="1"/>
   </cols>
@@ -1605,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1661,6 +1838,72 @@
       </c>
       <c r="C6" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1673,7 +1916,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1689,10 +1932,10 @@
         <v>48</v>
       </c>
       <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
         <v>86</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
       </c>
       <c r="D1" t="s">
         <v>49</v>
@@ -1703,10 +1946,10 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
         <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>50</v>
@@ -1714,13 +1957,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
         <v>90</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>50</v>
@@ -1728,13 +1971,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
       </c>
       <c r="D4" t="s">
         <v>50</v>
@@ -1742,13 +1985,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
       </c>
       <c r="D5" t="s">
         <v>50</v>
@@ -1756,13 +1999,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="s">
         <v>95</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>96</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
@@ -1770,13 +2013,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
@@ -1784,13 +2027,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
         <v>101</v>
-      </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
@@ -1798,13 +2041,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
         <v>103</v>
-      </c>
-      <c r="B9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
       </c>
       <c r="D9" t="s">
         <v>50</v>
@@ -1812,13 +2055,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
         <v>50</v>
@@ -1826,13 +2069,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
         <v>106</v>
       </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
         <v>50</v>
@@ -1840,13 +2083,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
         <v>108</v>
-      </c>
-      <c r="B12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" t="s">
-        <v>109</v>
       </c>
       <c r="D12" t="s">
         <v>50</v>
@@ -1854,13 +2097,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" t="s">
         <v>50</v>
@@ -1868,13 +2111,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" t="s">
         <v>111</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>113</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
mapped tags to tbs subject for ontario
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/NonGeoLookupTables.xlsx
+++ b/FME_files/LOOKUP_TABLES/NonGeoLookupTables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA98F4F-2418-45D8-851C-0ED6A9BB6C71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87306B70-DAFC-432C-BB40-4B6FDA41B1B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25965" yWindow="17700" windowWidth="22710" windowHeight="14445" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="15140" windowHeight="9630" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format_TBS" sheetId="1" r:id="rId1"/>
     <sheet name="Update_TBS" sheetId="2" r:id="rId2"/>
     <sheet name="ResourceType_TBS" sheetId="3" r:id="rId3"/>
-    <sheet name="SubjectNTopic_TBS" sheetId="4" r:id="rId4"/>
+    <sheet name="Subject_TBS_ON" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="288">
   <si>
     <t>TBS_value</t>
   </si>
@@ -294,87 +294,36 @@
     <t>guide</t>
   </si>
   <si>
-    <t>TBS_topic</t>
-  </si>
-  <si>
-    <t>TBS_subject</t>
-  </si>
-  <si>
-    <t>society</t>
-  </si>
-  <si>
     <t>society_and_culture</t>
   </si>
   <si>
-    <t>sante</t>
-  </si>
-  <si>
     <t>health</t>
   </si>
   <si>
     <t>health_and_safety</t>
   </si>
   <si>
-    <t>societe-culture</t>
-  </si>
-  <si>
-    <t>tourisme-sports-loisirs</t>
-  </si>
-  <si>
-    <t>economie-entreprises</t>
-  </si>
-  <si>
-    <t>economy</t>
-  </si>
-  <si>
     <t>economics_and_industry</t>
   </si>
   <si>
-    <t>environnement-ressources-naturelles-energie</t>
-  </si>
-  <si>
     <t>environment</t>
   </si>
   <si>
     <t>nature_and_environment</t>
   </si>
   <si>
-    <t>politiques-sociales</t>
-  </si>
-  <si>
     <t>government_and_politics</t>
   </si>
   <si>
-    <t>education-recherche</t>
-  </si>
-  <si>
     <t>education_and_training</t>
   </si>
   <si>
-    <t>gouvernement-finances</t>
-  </si>
-  <si>
-    <t>infrastructures</t>
-  </si>
-  <si>
-    <t>structure</t>
-  </si>
-  <si>
-    <t>loi-justice-securite-publique</t>
-  </si>
-  <si>
     <t>law</t>
   </si>
   <si>
     <t>transport</t>
   </si>
   <si>
-    <t>agriculture-alimentation</t>
-  </si>
-  <si>
-    <t>farming</t>
-  </si>
-  <si>
     <t>agriculture</t>
   </si>
   <si>
@@ -448,6 +397,510 @@
   </si>
   <si>
     <t>information</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>agriculture and food</t>
+  </si>
+  <si>
+    <t>alternate species</t>
+  </si>
+  <si>
+    <t>annual report</t>
+  </si>
+  <si>
+    <t>ignore</t>
+  </si>
+  <si>
+    <t>arts and culture</t>
+  </si>
+  <si>
+    <t>arts_music_literature</t>
+  </si>
+  <si>
+    <t>beef</t>
+  </si>
+  <si>
+    <t>benefits</t>
+  </si>
+  <si>
+    <t>breeding</t>
+  </si>
+  <si>
+    <t>business and economy</t>
+  </si>
+  <si>
+    <t>calving</t>
+  </si>
+  <si>
+    <t>cantor</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t>carpool</t>
+  </si>
+  <si>
+    <t>cases</t>
+  </si>
+  <si>
+    <t>child care</t>
+  </si>
+  <si>
+    <t>citizen science</t>
+  </si>
+  <si>
+    <t>clergy</t>
+  </si>
+  <si>
+    <t>commute</t>
+  </si>
+  <si>
+    <t>coronavirus</t>
+  </si>
+  <si>
+    <t>correctional institutions</t>
+  </si>
+  <si>
+    <t>corrections</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>covid-19</t>
+  </si>
+  <si>
+    <t>covid-19 testing locations</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>culture and recreation</t>
+  </si>
+  <si>
+    <t>culture et loisirs</t>
+  </si>
+  <si>
+    <t>dairy</t>
+  </si>
+  <si>
+    <t>denning</t>
+  </si>
+  <si>
+    <t>dépistage de la covid-19</t>
+  </si>
+  <si>
+    <t>détenus</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>données ontario</t>
+  </si>
+  <si>
+    <t>driving and roads</t>
+  </si>
+  <si>
+    <t>écoles</t>
+  </si>
+  <si>
+    <t>économie et affaires</t>
+  </si>
+  <si>
+    <t>economy and business</t>
+  </si>
+  <si>
+    <t>education and training</t>
+  </si>
+  <si>
+    <t>éducation et formation</t>
+  </si>
+  <si>
+    <t>elder</t>
+  </si>
+  <si>
+    <t>elderly</t>
+  </si>
+  <si>
+    <t>élémentaire</t>
+  </si>
+  <si>
+    <t>elementary</t>
+  </si>
+  <si>
+    <t>emrb</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>environment and energy</t>
+  </si>
+  <si>
+    <t>science_and_technology</t>
+  </si>
+  <si>
+    <t>environment and natural resources</t>
+  </si>
+  <si>
+    <t>environnement et énergie</t>
+  </si>
+  <si>
+    <t>environnement et richesses naturelles</t>
+  </si>
+  <si>
+    <t>établissements correctionnels</t>
+  </si>
+  <si>
+    <t>état</t>
+  </si>
+  <si>
+    <t>fair market value</t>
+  </si>
+  <si>
+    <t>fawning</t>
+  </si>
+  <si>
+    <t>feeding</t>
+  </si>
+  <si>
+    <t>fisheries</t>
+  </si>
+  <si>
+    <t>fishing</t>
+  </si>
+  <si>
+    <t>forest management planning</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>gasoline</t>
+  </si>
+  <si>
+    <t>general habitat</t>
+  </si>
+  <si>
+    <t>gouvernement</t>
+  </si>
+  <si>
+    <t>gouvernement et finances</t>
+  </si>
+  <si>
+    <t>government</t>
+  </si>
+  <si>
+    <t>government and finance</t>
+  </si>
+  <si>
+    <t>guaranteed annual income system</t>
+  </si>
+  <si>
+    <t>health and wellness</t>
+  </si>
+  <si>
+    <t>home and community</t>
+  </si>
+  <si>
+    <t>hôpitaux</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>housing communities and social support</t>
+  </si>
+  <si>
+    <t>imam</t>
+  </si>
+  <si>
+    <t>impôt sur le revenu</t>
+  </si>
+  <si>
+    <t>impôts et avantages fiscaux</t>
+  </si>
+  <si>
+    <t>income tax</t>
+  </si>
+  <si>
+    <t>infrastructure and transportation</t>
+  </si>
+  <si>
+    <t>infrastructure et transport</t>
+  </si>
+  <si>
+    <t>inland lakes</t>
+  </si>
+  <si>
+    <t>inmates</t>
+  </si>
+  <si>
+    <t>jobs and employment</t>
+  </si>
+  <si>
+    <t>labour</t>
+  </si>
+  <si>
+    <t>junior</t>
+  </si>
+  <si>
+    <t>justice and public safety</t>
+  </si>
+  <si>
+    <t>lacs</t>
+  </si>
+  <si>
+    <t>lakes</t>
+  </si>
+  <si>
+    <t>lamb</t>
+  </si>
+  <si>
+    <t>law and safety</t>
+  </si>
+  <si>
+    <t>livestock</t>
+  </si>
+  <si>
+    <t>logement collectivités et soutien social</t>
+  </si>
+  <si>
+    <t>lois et sécurité</t>
+  </si>
+  <si>
+    <t>mariage</t>
+  </si>
+  <si>
+    <t>market value</t>
+  </si>
+  <si>
+    <t>marriage</t>
+  </si>
+  <si>
+    <t>marriage officiant</t>
+  </si>
+  <si>
+    <t>migration</t>
+  </si>
+  <si>
+    <t>minister</t>
+  </si>
+  <si>
+    <t>missing persons</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>nesting birds</t>
+  </si>
+  <si>
+    <t>nesting reptiles</t>
+  </si>
+  <si>
+    <t>nesting site</t>
+  </si>
+  <si>
+    <t>northern health programs</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>nursery</t>
+  </si>
+  <si>
+    <t>officiant</t>
+  </si>
+  <si>
+    <t>old age security</t>
+  </si>
+  <si>
+    <t>opp annual report</t>
+  </si>
+  <si>
+    <t>owb</t>
+  </si>
+  <si>
+    <t>parking lots</t>
+  </si>
+  <si>
+    <t>pastor</t>
+  </si>
+  <si>
+    <t>payroll deduction</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>poultry</t>
+  </si>
+  <si>
+    <t>prêtre</t>
+  </si>
+  <si>
+    <t>prices</t>
+  </si>
+  <si>
+    <t>priest</t>
+  </si>
+  <si>
+    <t>program funding</t>
+  </si>
+  <si>
+    <t>propane</t>
+  </si>
+  <si>
+    <t>puits</t>
+  </si>
+  <si>
+    <t>rabbi</t>
+  </si>
+  <si>
+    <t>rates</t>
+  </si>
+  <si>
+    <t>régions rurales et du nord</t>
+  </si>
+  <si>
+    <t>regulations</t>
+  </si>
+  <si>
+    <t>resting</t>
+  </si>
+  <si>
+    <t>reverend</t>
+  </si>
+  <si>
+    <t>rules</t>
+  </si>
+  <si>
+    <t>rural and north</t>
+  </si>
+  <si>
+    <t>santé</t>
+  </si>
+  <si>
+    <t>santé et bien-être</t>
+  </si>
+  <si>
+    <t>schools</t>
+  </si>
+  <si>
+    <t>secondaire</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>seed collection</t>
+  </si>
+  <si>
+    <t>seed deployment</t>
+  </si>
+  <si>
+    <t>seed zone</t>
+  </si>
+  <si>
+    <t>seniors</t>
+  </si>
+  <si>
+    <t>services correctionnels</t>
+  </si>
+  <si>
+    <t>sheep</t>
+  </si>
+  <si>
+    <t>sikh</t>
+  </si>
+  <si>
+    <t>staging</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>swine</t>
+  </si>
+  <si>
+    <t>taux</t>
+  </si>
+  <si>
+    <t>taxes</t>
+  </si>
+  <si>
+    <t>taxes and benefits</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>travail et emploi</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>travel and recreation</t>
+  </si>
+  <si>
+    <t>travel corridor</t>
+  </si>
+  <si>
+    <t>tree seed</t>
+  </si>
+  <si>
+    <t>underserviced area programs</t>
+  </si>
+  <si>
+    <t>urgent demands for records</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>volailles</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>water quality</t>
+  </si>
+  <si>
+    <t>watershed</t>
+  </si>
+  <si>
+    <t>wedding</t>
+  </si>
+  <si>
+    <t>wells</t>
+  </si>
+  <si>
+    <t>wildlife</t>
+  </si>
+  <si>
+    <t>wintering</t>
+  </si>
+  <si>
+    <t>tag_value</t>
+  </si>
+  <si>
+    <t>subject_value</t>
   </si>
 </sst>
 </file>
@@ -1292,128 +1745,128 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
         <v>26</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B50" t="s">
         <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
         <v>43</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
         <v>42</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
         <v>18</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1619,7 +2072,7 @@
         <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1630,7 +2083,7 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1641,7 +2094,7 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1652,29 +2105,29 @@
         <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1685,40 +2138,40 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
         <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -1729,29 +2182,29 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1763,7 +2216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DA827-7F8F-427A-89AE-B21D8717466C}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1848,62 +2301,62 @@
         <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1912,215 +2365,1617 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859D5EAD-7742-45A1-BF94-958933ADEE28}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DC00A4-140D-49DA-BDB7-780ECFA36618}">
+  <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.1796875" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>286</v>
       </c>
       <c r="B1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>163</v>
+      </c>
+      <c r="B48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>168</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>171</v>
+      </c>
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>172</v>
+      </c>
+      <c r="B64" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>174</v>
+      </c>
+      <c r="B67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>175</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>176</v>
+      </c>
+      <c r="B69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>177</v>
+      </c>
+      <c r="B70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>178</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>179</v>
+      </c>
+      <c r="B72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>183</v>
+      </c>
+      <c r="B76" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>185</v>
+      </c>
+      <c r="B78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>86</v>
       </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B84" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>189</v>
+      </c>
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>190</v>
+      </c>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>191</v>
+      </c>
+      <c r="B87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>192</v>
+      </c>
+      <c r="B88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>193</v>
+      </c>
+      <c r="B89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>194</v>
+      </c>
+      <c r="B90" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>194</v>
+      </c>
+      <c r="B91" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>195</v>
+      </c>
+      <c r="B92" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>195</v>
+      </c>
+      <c r="B93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>196</v>
+      </c>
+      <c r="B94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>197</v>
+      </c>
+      <c r="B95" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>197</v>
+      </c>
+      <c r="B96" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>198</v>
+      </c>
+      <c r="B97" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>199</v>
+      </c>
+      <c r="B98" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>200</v>
+      </c>
+      <c r="B99" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>201</v>
+      </c>
+      <c r="B100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>202</v>
+      </c>
+      <c r="B101" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>205</v>
+      </c>
+      <c r="B103" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>207</v>
+      </c>
+      <c r="B105" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>208</v>
+      </c>
+      <c r="B106" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>209</v>
+      </c>
+      <c r="B107" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>210</v>
+      </c>
+      <c r="B108" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>212</v>
+      </c>
+      <c r="B110" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>214</v>
+      </c>
+      <c r="B113" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>215</v>
+      </c>
+      <c r="B114" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>215</v>
+      </c>
+      <c r="B115" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>216</v>
+      </c>
+      <c r="B116" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>216</v>
+      </c>
+      <c r="B117" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>217</v>
+      </c>
+      <c r="B118" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>218</v>
+      </c>
+      <c r="B119" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>218</v>
+      </c>
+      <c r="B120" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>219</v>
+      </c>
+      <c r="B121" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>220</v>
+      </c>
+      <c r="B122" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>221</v>
+      </c>
+      <c r="B123" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>222</v>
+      </c>
+      <c r="B124" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>223</v>
+      </c>
+      <c r="B125" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>224</v>
+      </c>
+      <c r="B126" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>225</v>
+      </c>
+      <c r="B127" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>226</v>
+      </c>
+      <c r="B128" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>227</v>
+      </c>
+      <c r="B129" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>228</v>
+      </c>
+      <c r="B130" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>229</v>
+      </c>
+      <c r="B131" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>230</v>
+      </c>
+      <c r="B132" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>231</v>
+      </c>
+      <c r="B133" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>232</v>
+      </c>
+      <c r="B134" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>232</v>
+      </c>
+      <c r="B135" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>233</v>
+      </c>
+      <c r="B136" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>234</v>
+      </c>
+      <c r="B137" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>235</v>
+      </c>
+      <c r="B138" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>236</v>
+      </c>
+      <c r="B139" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>236</v>
+      </c>
+      <c r="B140" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>237</v>
+      </c>
+      <c r="B141" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>238</v>
+      </c>
+      <c r="B142" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>238</v>
+      </c>
+      <c r="B143" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B144" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>240</v>
+      </c>
+      <c r="B145" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>241</v>
+      </c>
+      <c r="B146" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>242</v>
+      </c>
+      <c r="B147" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>242</v>
+      </c>
+      <c r="B148" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>243</v>
+      </c>
+      <c r="B149" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>243</v>
+      </c>
+      <c r="B150" t="s">
         <v>91</v>
       </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>244</v>
+      </c>
+      <c r="B151" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>245</v>
+      </c>
+      <c r="B152" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>246</v>
+      </c>
+      <c r="B153" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>247</v>
+      </c>
+      <c r="B154" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>247</v>
+      </c>
+      <c r="B155" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>248</v>
+      </c>
+      <c r="B156" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>249</v>
+      </c>
+      <c r="B157" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>250</v>
+      </c>
+      <c r="B158" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>251</v>
+      </c>
+      <c r="B159" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>252</v>
+      </c>
+      <c r="B160" t="s">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>253</v>
+      </c>
+      <c r="B161" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>254</v>
+      </c>
+      <c r="B162" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>255</v>
+      </c>
+      <c r="B163" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>256</v>
+      </c>
+      <c r="B164" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>257</v>
+      </c>
+      <c r="B165" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>258</v>
+      </c>
+      <c r="B166" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>259</v>
+      </c>
+      <c r="B167" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>260</v>
+      </c>
+      <c r="B168" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>261</v>
+      </c>
+      <c r="B169" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>261</v>
+      </c>
+      <c r="B170" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>262</v>
+      </c>
+      <c r="B171" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>263</v>
+      </c>
+      <c r="B172" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>264</v>
+      </c>
+      <c r="B173" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>265</v>
+      </c>
+      <c r="B174" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>265</v>
+      </c>
+      <c r="B175" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>266</v>
+      </c>
+      <c r="B176" t="s">
         <v>88</v>
       </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>266</v>
+      </c>
+      <c r="B177" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>267</v>
+      </c>
+      <c r="B178" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>268</v>
+      </c>
+      <c r="B179" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>269</v>
+      </c>
+      <c r="B180" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>270</v>
+      </c>
+      <c r="B181" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>271</v>
+      </c>
+      <c r="B182" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>272</v>
+      </c>
+      <c r="B183" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>272</v>
+      </c>
+      <c r="B184" t="s">
         <v>94</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>272</v>
+      </c>
+      <c r="B185" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>273</v>
+      </c>
+      <c r="B186" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>274</v>
+      </c>
+      <c r="B187" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>275</v>
+      </c>
+      <c r="B188" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>276</v>
+      </c>
+      <c r="B189" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>277</v>
+      </c>
+      <c r="B190" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>278</v>
+      </c>
+      <c r="B191" t="s">
         <v>95</v>
       </c>
-      <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>279</v>
+      </c>
+      <c r="B192" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>279</v>
+      </c>
+      <c r="B193" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>280</v>
+      </c>
+      <c r="B194" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>280</v>
+      </c>
+      <c r="B195" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>281</v>
+      </c>
+      <c r="B196" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>282</v>
+      </c>
+      <c r="B197" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>283</v>
+      </c>
+      <c r="B198" t="s">
         <v>88</v>
       </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>284</v>
+      </c>
+      <c r="B199" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>285</v>
+      </c>
+      <c r="B200" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>